<commit_message>
TestNG program by using Excel data
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -22,7 +22,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Admin</t>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>Admin1</t>
+  </si>
+  <si>
+    <t>admin908</t>
   </si>
 </sst>
 </file>
@@ -364,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,10 +391,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>